<commit_message>
VERY CLOSE TO FINISH PRINT BEFORE PAGE
ONLY NEED TO HANDLE FIRST ROUND PRINT NOW
</commit_message>
<xml_diff>
--- a/Fwd__bowling_ver10/rawData/data/before_Sheet.xlsx
+++ b/Fwd__bowling_ver10/rawData/data/before_Sheet.xlsx
@@ -16,6 +16,9 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">גיליון1!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">גיליון1!$A:$K,גיליון1!$1:$47</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">גיליון2!$A:$K,גיליון2!$1:$47</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">גיליון3!$A:$K,גיליון3!$1:$47</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">גיליון4!$A:$K,גיליון4!$1:$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">גיליון5!$A:$K,גיליון5!$1:$47</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="61">
   <si>
     <t>אגודת כדורת - אשדוד</t>
   </si>
@@ -121,19 +124,10 @@
     <t>07.06.16</t>
   </si>
   <si>
-    <t>ון קופם</t>
-  </si>
-  <si>
-    <t>4 + 5</t>
-  </si>
-  <si>
     <t>קבוצה 5</t>
   </si>
   <si>
     <t>חתימת קפטן קבוצה 5:</t>
-  </si>
-  <si>
-    <t>SKS</t>
   </si>
   <si>
     <t xml:space="preserve">פרגמין גולן </t>
@@ -154,6 +148,69 @@
   <si>
     <t>_x000D_
 גגג</t>
+  </si>
+  <si>
+    <t>שלום לכולם אנחנו מתחילים בפיילוט עם התוכנה החדשה</t>
+  </si>
+  <si>
+    <t>קבוצה 2</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 2:</t>
+  </si>
+  <si>
+    <t>קבוצה 1</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 1:</t>
+  </si>
+  <si>
+    <t>3 + 4</t>
+  </si>
+  <si>
+    <t>5 + 6</t>
+  </si>
+  <si>
+    <t>7 + 8</t>
+  </si>
+  <si>
+    <t>9 + 10</t>
+  </si>
+  <si>
+    <t>קבוצה 3</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 3:</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 6:</t>
+  </si>
+  <si>
+    <t>קבוצה 6</t>
+  </si>
+  <si>
+    <t>קבוצה 7</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 8:</t>
+  </si>
+  <si>
+    <t>קבוצה 8</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 7:</t>
+  </si>
+  <si>
+    <t>קבוצה 9</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 10:</t>
+  </si>
+  <si>
+    <t>קבוצה 10</t>
+  </si>
+  <si>
+    <t>חתימת קפטן קבוצה 9:</t>
   </si>
 </sst>
 </file>
@@ -361,17 +418,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,23 +442,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A27" sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -710,33 +767,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="14"/>
       <c r="D4">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
       <c r="H4" s="3" t="s">
         <v>4</v>
       </c>
@@ -745,19 +799,16 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="14"/>
       <c r="D5">
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
       <c r="H5" s="3" t="s">
         <v>5</v>
       </c>
@@ -766,19 +817,16 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="14"/>
       <c r="D6">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="3" t="s">
         <v>6</v>
       </c>
@@ -787,24 +835,21 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="14"/>
       <c r="D7">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1">
@@ -819,7 +864,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -829,35 +874,35 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>202.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18">
       <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="14"/>
       <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="14"/>
       <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="14"/>
       <c r="I12">
         <v>0</v>
       </c>
@@ -880,10 +925,10 @@
       <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="10" t="s">
         <v>18</v>
       </c>
@@ -902,13 +947,13 @@
     </row>
     <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B15" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="10"/>
@@ -919,13 +964,13 @@
     </row>
     <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B16" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C16" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="10"/>
@@ -936,15 +981,15 @@
     </row>
     <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B17" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C17" s="10">
-        <v>32</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="24"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -957,7 +1002,7 @@
       </c>
       <c r="C18" s="10">
         <f>SUM(C15:C17)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>24</v>
@@ -970,60 +1015,60 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10">
         <f>SUM(G19:I19)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1">
-      <c r="B24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="B24" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="15" thickBot="1">
       <c r="A25" s="4"/>
@@ -1041,30 +1086,30 @@
     <row r="26" spans="1:11" ht="15" thickTop="1"/>
     <row r="27" spans="1:11" ht="18">
       <c r="E27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="14"/>
       <c r="I27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="14"/>
       <c r="I28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="14"/>
       <c r="I29">
         <v>0</v>
       </c>
@@ -1087,10 +1132,10 @@
       <c r="C31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="10" t="s">
         <v>18</v>
       </c>
@@ -1109,13 +1154,13 @@
     </row>
     <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B32" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="10"/>
@@ -1126,13 +1171,13 @@
     </row>
     <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B33" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C33" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="10"/>
@@ -1143,15 +1188,15 @@
     </row>
     <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B34" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C34" s="10">
-        <v>32</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="24"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -1164,7 +1209,7 @@
       </c>
       <c r="C35" s="10">
         <f>SUM(C32:C34)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>22</v>
@@ -1177,60 +1222,60 @@
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J36" s="10">
         <f>SUM(G36:I36)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="15" thickBot="1">
-      <c r="B41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="B41" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
     </row>
     <row r="42" spans="1:11" ht="15" thickBot="1">
       <c r="A42" s="4"/>
@@ -1247,28 +1292,38 @@
     </row>
     <row r="43" spans="1:11" ht="15" thickTop="1"/>
     <row r="44" spans="1:11" ht="23.25">
-      <c r="A44" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
+      <c r="A44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G27:H27"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
@@ -1279,22 +1334,12 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1306,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1317,33 +1362,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="14"/>
       <c r="D4">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
       <c r="H4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1352,19 +1394,16 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="14"/>
       <c r="D5">
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
       <c r="H5" s="13" t="s">
         <v>5</v>
       </c>
@@ -1373,45 +1412,39 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="14"/>
       <c r="D6">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="14"/>
       <c r="D7">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1">
@@ -1426,7 +1459,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1436,35 +1469,35 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>202.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18">
       <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="14"/>
       <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="14"/>
       <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="14"/>
       <c r="I12">
         <v>0</v>
       </c>
@@ -1487,10 +1520,10 @@
       <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1509,13 +1542,13 @@
     </row>
     <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B15" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="10"/>
@@ -1526,13 +1559,13 @@
     </row>
     <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B16" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C16" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="10"/>
@@ -1543,15 +1576,15 @@
     </row>
     <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B17" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C17" s="10">
-        <v>32</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="24"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1564,7 +1597,7 @@
       </c>
       <c r="C18" s="10">
         <f>SUM(C15:C17)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>24</v>
@@ -1577,60 +1610,60 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10">
         <f>SUM(G19:I19)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1">
-      <c r="B24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="B24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="15" thickBot="1">
       <c r="A25" s="4"/>
@@ -1648,30 +1681,30 @@
     <row r="26" spans="1:11" ht="15" thickTop="1"/>
     <row r="27" spans="1:11" ht="18">
       <c r="E27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="14"/>
       <c r="I27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="14"/>
       <c r="I28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="14"/>
       <c r="I29">
         <v>0</v>
       </c>
@@ -1694,10 +1727,10 @@
       <c r="C31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="10" t="s">
         <v>18</v>
       </c>
@@ -1716,13 +1749,13 @@
     </row>
     <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B32" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="10"/>
@@ -1733,13 +1766,13 @@
     </row>
     <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B33" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C33" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="10"/>
@@ -1750,15 +1783,15 @@
     </row>
     <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B34" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C34" s="10">
-        <v>32</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="24"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -1771,7 +1804,7 @@
       </c>
       <c r="C35" s="10">
         <f>SUM(C32:C34)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>22</v>
@@ -1784,60 +1817,60 @@
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J36" s="10">
         <f>SUM(G36:I36)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="15" thickBot="1">
-      <c r="B41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="B41" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
     </row>
     <row r="42" spans="1:11" ht="15" thickBot="1">
       <c r="A42" s="4"/>
@@ -1854,28 +1887,40 @@
     </row>
     <row r="43" spans="1:11" ht="15" thickTop="1"/>
     <row r="44" spans="1:11" ht="23.25">
-      <c r="A44" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
+      <c r="A44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:H24"/>
     <mergeCell ref="G11:H11"/>
@@ -1884,26 +1929,16 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="74" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1911,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1922,33 +1957,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="14"/>
       <c r="D4">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
       <c r="H4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1957,19 +1989,16 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="14"/>
       <c r="D5">
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
       <c r="H5" s="13" t="s">
         <v>5</v>
       </c>
@@ -1978,45 +2007,39 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="14"/>
       <c r="D6">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="14"/>
       <c r="D7">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1">
@@ -2031,7 +2054,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2041,35 +2064,35 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>202.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18">
       <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="14"/>
       <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="14"/>
       <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="14"/>
       <c r="I12">
         <v>0</v>
       </c>
@@ -2092,10 +2115,10 @@
       <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="10" t="s">
         <v>18</v>
       </c>
@@ -2114,13 +2137,13 @@
     </row>
     <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B15" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="10"/>
@@ -2131,13 +2154,13 @@
     </row>
     <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B16" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C16" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="10"/>
@@ -2148,15 +2171,15 @@
     </row>
     <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B17" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C17" s="10">
-        <v>32</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="24"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -2169,7 +2192,7 @@
       </c>
       <c r="C18" s="10">
         <f>SUM(C15:C17)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>24</v>
@@ -2182,60 +2205,60 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10">
         <f>SUM(G19:I19)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1">
-      <c r="B24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="B24" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="15" thickBot="1">
       <c r="A25" s="4"/>
@@ -2253,30 +2276,30 @@
     <row r="26" spans="1:11" ht="15" thickTop="1"/>
     <row r="27" spans="1:11" ht="18">
       <c r="E27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="14"/>
       <c r="I27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="14"/>
       <c r="I28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="14"/>
       <c r="I29">
         <v>0</v>
       </c>
@@ -2299,10 +2322,10 @@
       <c r="C31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="10" t="s">
         <v>18</v>
       </c>
@@ -2321,13 +2344,13 @@
     </row>
     <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B32" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="10"/>
@@ -2338,13 +2361,13 @@
     </row>
     <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B33" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C33" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="10"/>
@@ -2355,15 +2378,15 @@
     </row>
     <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B34" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C34" s="10">
-        <v>32</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="24"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -2376,7 +2399,7 @@
       </c>
       <c r="C35" s="10">
         <f>SUM(C32:C34)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>22</v>
@@ -2389,60 +2412,60 @@
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J36" s="10">
         <f>SUM(G36:I36)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="15" thickBot="1">
-      <c r="B41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="B41" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
     </row>
     <row r="42" spans="1:11" ht="15" thickBot="1">
       <c r="A42" s="4"/>
@@ -2459,28 +2482,40 @@
     </row>
     <row r="43" spans="1:11" ht="15" thickTop="1"/>
     <row r="44" spans="1:11" ht="23.25">
-      <c r="A44" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
+      <c r="A44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:H24"/>
     <mergeCell ref="G11:H11"/>
@@ -2489,26 +2524,16 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="74" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2516,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2527,33 +2552,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="14"/>
       <c r="D4">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
       <c r="H4" s="13" t="s">
         <v>4</v>
       </c>
@@ -2562,19 +2584,16 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="14"/>
       <c r="D5">
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
       <c r="H5" s="13" t="s">
         <v>5</v>
       </c>
@@ -2583,45 +2602,39 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="14"/>
       <c r="D6">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="14"/>
       <c r="D7">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1">
@@ -2636,7 +2649,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2646,35 +2659,35 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>202.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18">
       <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="14"/>
       <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="14"/>
       <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="14"/>
       <c r="I12">
         <v>0</v>
       </c>
@@ -2697,10 +2710,10 @@
       <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="10" t="s">
         <v>18</v>
       </c>
@@ -2719,13 +2732,13 @@
     </row>
     <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B15" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="10"/>
@@ -2736,13 +2749,13 @@
     </row>
     <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B16" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C16" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="10"/>
@@ -2753,15 +2766,15 @@
     </row>
     <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B17" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C17" s="10">
-        <v>32</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="24"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -2774,7 +2787,7 @@
       </c>
       <c r="C18" s="10">
         <f>SUM(C15:C17)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>24</v>
@@ -2787,60 +2800,60 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10">
         <f>SUM(G19:I19)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1">
-      <c r="B24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="B24" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="15" thickBot="1">
       <c r="A25" s="4"/>
@@ -2858,30 +2871,30 @@
     <row r="26" spans="1:11" ht="15" thickTop="1"/>
     <row r="27" spans="1:11" ht="18">
       <c r="E27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="14"/>
       <c r="I27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="14"/>
       <c r="I28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="14"/>
       <c r="I29">
         <v>0</v>
       </c>
@@ -2904,10 +2917,10 @@
       <c r="C31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="10" t="s">
         <v>18</v>
       </c>
@@ -2926,13 +2939,13 @@
     </row>
     <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B32" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="10"/>
@@ -2943,13 +2956,13 @@
     </row>
     <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B33" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C33" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="10"/>
@@ -2960,15 +2973,15 @@
     </row>
     <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B34" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C34" s="10">
-        <v>32</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="24"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -2981,7 +2994,7 @@
       </c>
       <c r="C35" s="10">
         <f>SUM(C32:C34)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>22</v>
@@ -2994,60 +3007,60 @@
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J36" s="10">
         <f>SUM(G36:I36)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="15" thickBot="1">
-      <c r="B41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="B41" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
     </row>
     <row r="42" spans="1:11" ht="15" thickBot="1">
       <c r="A42" s="4"/>
@@ -3064,28 +3077,40 @@
     </row>
     <row r="43" spans="1:11" ht="15" thickTop="1"/>
     <row r="44" spans="1:11" ht="23.25">
-      <c r="A44" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
+      <c r="A44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:H24"/>
     <mergeCell ref="G11:H11"/>
@@ -3094,26 +3119,16 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="74" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3121,8 +3136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3132,33 +3147,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="D1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="14"/>
       <c r="D4">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
       <c r="H4" s="13" t="s">
         <v>4</v>
       </c>
@@ -3167,19 +3179,16 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="14"/>
       <c r="D5">
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
       <c r="H5" s="13" t="s">
         <v>5</v>
       </c>
@@ -3188,45 +3197,39 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="14"/>
       <c r="D6">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="14"/>
       <c r="D7">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1">
@@ -3241,7 +3244,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -3251,35 +3254,35 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>202.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18">
       <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="14"/>
       <c r="I10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="14"/>
       <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="14"/>
       <c r="I12">
         <v>0</v>
       </c>
@@ -3302,10 +3305,10 @@
       <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="10" t="s">
         <v>18</v>
       </c>
@@ -3324,13 +3327,13 @@
     </row>
     <row r="15" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B15" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="10"/>
@@ -3341,13 +3344,13 @@
     </row>
     <row r="16" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B16" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C16" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="10"/>
@@ -3358,15 +3361,15 @@
     </row>
     <row r="17" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B17" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C17" s="10">
-        <v>32</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="24"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -3379,7 +3382,7 @@
       </c>
       <c r="C18" s="10">
         <f>SUM(C15:C17)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>24</v>
@@ -3392,60 +3395,60 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I19" s="10">
         <f>C18</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J19" s="10">
         <f>SUM(G19:I19)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1">
-      <c r="B24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="B24" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:11" ht="15" thickBot="1">
       <c r="A25" s="4"/>
@@ -3463,30 +3466,30 @@
     <row r="26" spans="1:11" ht="15" thickTop="1"/>
     <row r="27" spans="1:11" ht="18">
       <c r="E27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="14"/>
       <c r="I27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="14"/>
       <c r="I28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="14"/>
       <c r="I29">
         <v>0</v>
       </c>
@@ -3509,10 +3512,10 @@
       <c r="C31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="10" t="s">
         <v>18</v>
       </c>
@@ -3531,13 +3534,13 @@
     </row>
     <row r="32" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B32" s="9">
-        <v>171.2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="10">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="10"/>
@@ -3548,13 +3551,13 @@
     </row>
     <row r="33" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B33" s="9">
-        <v>142.79</v>
+        <v>0</v>
       </c>
       <c r="C33" s="10">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="10"/>
@@ -3565,15 +3568,15 @@
     </row>
     <row r="34" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
       <c r="B34" s="9">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="C34" s="10">
-        <v>32</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="24"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -3586,7 +3589,7 @@
       </c>
       <c r="C35" s="10">
         <f>SUM(C32:C34)</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>22</v>
@@ -3599,60 +3602,60 @@
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I36" s="10">
         <f>C35</f>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J36" s="10">
         <f>SUM(G36:I36)</f>
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:11" ht="40.5" customHeight="1" thickBot="1">
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="15" thickBot="1">
-      <c r="B41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="B41" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
     </row>
     <row r="42" spans="1:11" ht="15" thickBot="1">
       <c r="A42" s="4"/>
@@ -3669,28 +3672,40 @@
     </row>
     <row r="43" spans="1:11" ht="15" thickTop="1"/>
     <row r="44" spans="1:11" ht="23.25">
-      <c r="A44" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
+      <c r="A44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D1:G2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:H24"/>
     <mergeCell ref="G11:H11"/>
@@ -3699,24 +3714,12 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>